<commit_message>
add .gitignore and update generated timetable outputs
</commit_message>
<xml_diff>
--- a/outputs/department_timetables/CSEA_1.xlsx
+++ b/outputs/department_timetables/CSEA_1.xlsx
@@ -704,20 +704,20 @@
         </is>
       </c>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" s="2" t="inlineStr">
-        <is>
-          <t>CS161 | Problem Solving through Programming | Dr. Sunil P V | C002</t>
-        </is>
-      </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
+      <c r="AG2" s="2" t="inlineStr">
+        <is>
+          <t>CS161 | Problem Solving through Programming | Dr. Sunil P V | C002</t>
+        </is>
+      </c>
       <c r="AM2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -970,6 +970,7 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="G6:N6"/>
+    <mergeCell ref="AG2:AL2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="I2:N2"/>
@@ -981,7 +982,6 @@
     <mergeCell ref="I3:N3"/>
     <mergeCell ref="G4:L4"/>
     <mergeCell ref="S3:X3"/>
-    <mergeCell ref="X2:AC2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>